<commit_message>
add vintages and output from full run
</commit_message>
<xml_diff>
--- a/Nowcasts/2025Q2/tables/nowcasts_2025Q2_Nr10_Np1_Nj0.xlsx
+++ b/Nowcasts/2025Q2/tables/nowcasts_2025Q2_Nr10_Np1_Nj0.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Row</t>
   </si>
@@ -22,6 +22,63 @@
   </si>
   <si>
     <t>2025-04-15</t>
+  </si>
+  <si>
+    <t>Prognose</t>
+  </si>
+  <si>
+    <t>surveys</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>turnover</t>
+  </si>
+  <si>
+    <t>financial</t>
+  </si>
+  <si>
+    <t>labor market</t>
+  </si>
+  <si>
+    <t>prices</t>
+  </si>
+  <si>
+    <t>national accounts</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>2025-03-30</t>
+  </si>
+  <si>
+    <t>2025-04-15</t>
+  </si>
+  <si>
+    <t>2025-04-30</t>
+  </si>
+  <si>
+    <t>2025-05-15</t>
+  </si>
+  <si>
+    <t>2025-05-30</t>
+  </si>
+  <si>
+    <t>2025-06-15</t>
+  </si>
+  <si>
+    <t>2025-06-30</t>
+  </si>
+  <si>
+    <t>2025-07-15</t>
   </si>
   <si>
     <t>Prognose</t>
@@ -97,60 +154,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K9"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.37890625" customWidth="true"/>
     <col min="2" max="2" width="13.64453125" customWidth="true"/>
-    <col min="3" max="3" width="6.98046875" customWidth="true"/>
-    <col min="4" max="4" width="9.77734375" customWidth="true"/>
-    <col min="5" max="5" width="6.1796875" customWidth="true"/>
-    <col min="6" max="6" width="7.98046875" customWidth="true"/>
-    <col min="7" max="7" width="7.84375" customWidth="true"/>
-    <col min="8" max="8" width="11.3125" customWidth="true"/>
-    <col min="9" max="9" width="5.77734375" customWidth="true"/>
+    <col min="3" max="3" width="14.24609375" customWidth="true"/>
+    <col min="4" max="4" width="14.24609375" customWidth="true"/>
+    <col min="5" max="5" width="15.1796875" customWidth="true"/>
+    <col min="6" max="6" width="15.24609375" customWidth="true"/>
+    <col min="7" max="7" width="15.24609375" customWidth="true"/>
+    <col min="8" max="8" width="15.24609375" customWidth="true"/>
+    <col min="9" max="9" width="16.24609375" customWidth="true"/>
     <col min="10" max="10" width="15.046875" customWidth="true"/>
-    <col min="11" max="11" width="7.7109375" customWidth="true"/>
+    <col min="11" max="11" width="15.24609375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0">
         <v>0.014386748655181247</v>
@@ -185,7 +242,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0">
         <v>0.45779160783153638</v>
@@ -216,6 +273,216 @@
       </c>
       <c r="K3" s="0">
         <v>-0.001798689103610529</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="0">
+        <v>0.36581984910544213</v>
+      </c>
+      <c r="C4" s="0">
+        <v>-0.12004503205611514</v>
+      </c>
+      <c r="D4" s="0">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0">
+        <v>1.4614836476838241e-07</v>
+      </c>
+      <c r="F4" s="0">
+        <v>-0.0031331993950290881</v>
+      </c>
+      <c r="G4" s="0">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0">
+        <v>-0.0056934384392859057</v>
+      </c>
+      <c r="I4" s="0">
+        <v>-0.04601571859244781</v>
+      </c>
+      <c r="J4" s="0">
+        <v>0.076485701710762341</v>
+      </c>
+      <c r="K4" s="0">
+        <v>0.0064297818976565835</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0.43333438878540254</v>
+      </c>
+      <c r="C5" s="0">
+        <v>-0.14632800143291763</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.12406236133514671</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0.029349786348602643</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0.074365154532043329</v>
+      </c>
+      <c r="G5" s="0">
+        <v>0.015564355340723996</v>
+      </c>
+      <c r="H5" s="0">
+        <v>-0.0024191573348651915</v>
+      </c>
+      <c r="I5" s="0">
+        <v>-0.022351874248269434</v>
+      </c>
+      <c r="J5" s="0">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0">
+        <v>-0.0047280848605040227</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="0">
+        <v>0.63321641702194564</v>
+      </c>
+      <c r="C6" s="0">
+        <v>0.32426033083005468</v>
+      </c>
+      <c r="D6" s="0">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0">
+        <v>0.013985236624663938</v>
+      </c>
+      <c r="F6" s="0">
+        <v>-0.015428036119258104</v>
+      </c>
+      <c r="G6" s="0">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0">
+        <v>-0.014634877408273739</v>
+      </c>
+      <c r="I6" s="0">
+        <v>-0.15204413115460266</v>
+      </c>
+      <c r="J6" s="0">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0">
+        <v>0.043743505463958998</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0">
+        <v>0.87042665462348712</v>
+      </c>
+      <c r="C7" s="0">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0">
+        <v>-0.056610392865325126</v>
+      </c>
+      <c r="E7" s="0">
+        <v>0.088362309754697499</v>
+      </c>
+      <c r="F7" s="0">
+        <v>0.20953061571349199</v>
+      </c>
+      <c r="G7" s="0">
+        <v>-0.008819344599250439</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0">
+        <v>0.015612610609752171</v>
+      </c>
+      <c r="J7" s="0">
+        <v>0</v>
+      </c>
+      <c r="K7" s="0">
+        <v>-0.010865561011824676</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="0">
+        <v>0.83694221399215962</v>
+      </c>
+      <c r="C8" s="0">
+        <v>-0.025334769451280513</v>
+      </c>
+      <c r="D8" s="0">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0.01680113233934637</v>
+      </c>
+      <c r="F8" s="0">
+        <v>-0.028357889233816411</v>
+      </c>
+      <c r="G8" s="0">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0.0014191378002149984</v>
+      </c>
+      <c r="I8" s="0">
+        <v>-0.00039821034206781371</v>
+      </c>
+      <c r="J8" s="0">
+        <v>0</v>
+      </c>
+      <c r="K8" s="0">
+        <v>0.002386158256275861</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="0">
+        <v>0.39311145717598134</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0">
+        <v>-0.16386961176621362</v>
+      </c>
+      <c r="E9" s="0">
+        <v>-0.05240481352532713</v>
+      </c>
+      <c r="F9" s="0">
+        <v>-0.24879078687711306</v>
+      </c>
+      <c r="G9" s="0">
+        <v>-0.015320445276329775</v>
+      </c>
+      <c r="H9" s="0">
+        <v>-0.00088015206441121241</v>
+      </c>
+      <c r="I9" s="0">
+        <v>-0.0026127127069326449</v>
+      </c>
+      <c r="J9" s="0">
+        <v>0</v>
+      </c>
+      <c r="K9" s="0">
+        <v>0.040047765400149204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>